<commit_message>
still waiting for all programming designations to be updated
</commit_message>
<xml_diff>
--- a/PEAR/PEAR Football/y2025/Spreads/spreads_tracker_week10.xlsx
+++ b/PEAR/PEAR Football/y2025/Spreads/spreads_tracker_week10.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P45"/>
+  <dimension ref="A1:P53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -716,40 +716,40 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Florida State</t>
+          <t>UConn</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Wake Forest</t>
+          <t>UAB</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>8.1</v>
+        <v>4.6</v>
       </c>
       <c r="E6" t="n">
-        <v>5.5</v>
+        <v>5</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Florida State -7.0</t>
+          <t>UConn -12.5</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Florida State -7</t>
+          <t>UConn -11.5</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Florida State -12.5</t>
+          <t>UConn -16.5</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>12.5</v>
+        <v>16.5</v>
       </c>
       <c r="J6" t="n">
-        <v>7</v>
+        <v>11.5</v>
       </c>
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr"/>
@@ -866,40 +866,40 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Troy</t>
+          <t>Florida State</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Arkansas State</t>
+          <t>Wake Forest</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>5.6</v>
+        <v>8.1</v>
       </c>
       <c r="E9" t="n">
-        <v>4.1</v>
+        <v>4</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Troy -7.0</t>
+          <t>Florida State -7.0</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Troy -7</t>
+          <t>Florida State -8.5</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Troy -11.1</t>
+          <t>Florida State -12.5</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>11.1</v>
+        <v>12.5</v>
       </c>
       <c r="J9" t="n">
-        <v>7</v>
+        <v>8.5</v>
       </c>
       <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr"/>
@@ -916,40 +916,40 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>UConn</t>
+          <t>Baylor</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>UAB</t>
+          <t>UCF</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>4.6</v>
+        <v>8.9</v>
       </c>
       <c r="E10" t="n">
         <v>4</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>UConn -12.5</t>
+          <t>Baylor -4.5</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>UConn -12.5</t>
+          <t>Baylor -5.5</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>UConn -16.5</t>
+          <t>Baylor -1.5</t>
         </is>
       </c>
       <c r="I10" t="n">
-        <v>16.5</v>
+        <v>1.5</v>
       </c>
       <c r="J10" t="n">
-        <v>12.5</v>
+        <v>5.5</v>
       </c>
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr"/>
@@ -1116,40 +1116,40 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Michigan</t>
+          <t>Troy</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Purdue</t>
+          <t>Arkansas State</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>6</v>
+        <v>5.6</v>
       </c>
       <c r="E14" t="n">
-        <v>3.600000000000001</v>
+        <v>3.6</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Michigan -20.5</t>
+          <t>Troy -7.0</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Michigan -20.5</t>
+          <t>Troy -7.5</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Michigan -24.1</t>
+          <t>Troy -11.1</t>
         </is>
       </c>
       <c r="I14" t="n">
-        <v>24.1</v>
+        <v>11.1</v>
       </c>
       <c r="J14" t="n">
-        <v>20.5</v>
+        <v>7.5</v>
       </c>
       <c r="K14" t="inlineStr"/>
       <c r="L14" t="inlineStr"/>
@@ -1216,40 +1216,40 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Iowa State</t>
+          <t>UL Monroe</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Arizona State</t>
+          <t>Old Dominion</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E16" t="n">
-        <v>3</v>
+        <v>3.199999999999999</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Iowa State -3.0</t>
+          <t>Old Dominion -14.0</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Iowa State -3</t>
+          <t>Old Dominion -14</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Iowa State -6.0</t>
+          <t>Old Dominion -17.2</t>
         </is>
       </c>
       <c r="I16" t="n">
-        <v>6</v>
+        <v>-17.2</v>
       </c>
       <c r="J16" t="n">
-        <v>3</v>
+        <v>-14</v>
       </c>
       <c r="K16" t="inlineStr"/>
       <c r="L16" t="inlineStr"/>
@@ -1266,40 +1266,40 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Baylor</t>
+          <t>Michigan</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>UCF</t>
+          <t>Purdue</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>8.9</v>
+        <v>6</v>
       </c>
       <c r="E17" t="n">
-        <v>3</v>
+        <v>3.100000000000001</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Baylor -4.5</t>
+          <t>Michigan -20.5</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Baylor -4.5</t>
+          <t>Michigan -21</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Baylor -1.5</t>
+          <t>Michigan -24.1</t>
         </is>
       </c>
       <c r="I17" t="n">
-        <v>1.5</v>
+        <v>24.1</v>
       </c>
       <c r="J17" t="n">
-        <v>4.5</v>
+        <v>21</v>
       </c>
       <c r="K17" t="inlineStr"/>
       <c r="L17" t="inlineStr"/>
@@ -1366,40 +1366,40 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Missouri State</t>
+          <t>Coastal Carolina</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Florida International</t>
+          <t>Marshall</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>5.1</v>
+        <v>4.9</v>
       </c>
       <c r="E19" t="n">
         <v>2.9</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Missouri State -2.5</t>
+          <t>Marshall -3.0</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Missouri State -3</t>
+          <t>Marshall -4</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Missouri State -5.9</t>
+          <t>Marshall -6.9</t>
         </is>
       </c>
       <c r="I19" t="n">
-        <v>5.9</v>
+        <v>-6.9</v>
       </c>
       <c r="J19" t="n">
-        <v>3</v>
+        <v>-4</v>
       </c>
       <c r="K19" t="inlineStr"/>
       <c r="L19" t="inlineStr"/>
@@ -1416,40 +1416,40 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Coastal Carolina</t>
+          <t>Boston College</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Marshall</t>
+          <t>Notre Dame</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>4.9</v>
+        <v>4.1</v>
       </c>
       <c r="E20" t="n">
-        <v>2.9</v>
+        <v>2.800000000000001</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Marshall -3.0</t>
+          <t>Notre Dame -27.5</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Marshall -4</t>
+          <t>Notre Dame -27.5</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Marshall -6.9</t>
+          <t>Notre Dame -30.3</t>
         </is>
       </c>
       <c r="I20" t="n">
-        <v>-6.9</v>
+        <v>-30.3</v>
       </c>
       <c r="J20" t="n">
-        <v>-4</v>
+        <v>-27.5</v>
       </c>
       <c r="K20" t="inlineStr"/>
       <c r="L20" t="inlineStr"/>
@@ -1466,40 +1466,40 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Boston College</t>
+          <t>Tennessee</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Notre Dame</t>
+          <t>Oklahoma</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>4.1</v>
+        <v>9.699999999999999</v>
       </c>
       <c r="E21" t="n">
-        <v>2.800000000000001</v>
+        <v>2.8</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Notre Dame -27.5</t>
+          <t>Tennessee -2.5</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Notre Dame -27.5</t>
+          <t>Tennessee -4</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Notre Dame -30.3</t>
+          <t>Tennessee -1.2</t>
         </is>
       </c>
       <c r="I21" t="n">
-        <v>-30.3</v>
+        <v>1.2</v>
       </c>
       <c r="J21" t="n">
-        <v>-27.5</v>
+        <v>4</v>
       </c>
       <c r="K21" t="inlineStr"/>
       <c r="L21" t="inlineStr"/>
@@ -1516,40 +1516,40 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Tennessee</t>
+          <t>Iowa State</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Oklahoma</t>
+          <t>Arizona State</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>9.699999999999999</v>
+        <v>9</v>
       </c>
       <c r="E22" t="n">
-        <v>2.8</v>
+        <v>2.5</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Tennessee -2.5</t>
+          <t>Iowa State -3.0</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Tennessee -4</t>
+          <t>Iowa State -3.5</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Tennessee -1.2</t>
+          <t>Iowa State -6.0</t>
         </is>
       </c>
       <c r="I22" t="n">
-        <v>1.2</v>
+        <v>6</v>
       </c>
       <c r="J22" t="n">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="K22" t="inlineStr"/>
       <c r="L22" t="inlineStr"/>
@@ -1566,40 +1566,40 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Oregon State</t>
+          <t>Stanford</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Washington State</t>
+          <t>Pittsburgh</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>5.9</v>
+        <v>5.1</v>
       </c>
       <c r="E23" t="n">
-        <v>2.8</v>
+        <v>2.5</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Washington State -3.0</t>
+          <t>Pittsburgh -15.5</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Washington State -3</t>
+          <t>Pittsburgh -14.5</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Washington State -5.8</t>
+          <t>Pittsburgh -17.0</t>
         </is>
       </c>
       <c r="I23" t="n">
-        <v>-5.8</v>
+        <v>-17</v>
       </c>
       <c r="J23" t="n">
-        <v>-3</v>
+        <v>-14.5</v>
       </c>
       <c r="K23" t="inlineStr"/>
       <c r="L23" t="inlineStr"/>
@@ -1616,40 +1616,40 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Illinois</t>
+          <t>Missouri State</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Rutgers</t>
+          <t>Florida International</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>8.1</v>
+        <v>5.1</v>
       </c>
       <c r="E24" t="n">
-        <v>2.300000000000001</v>
+        <v>2.4</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Illinois -10.5</t>
+          <t>Missouri State -2.5</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Illinois -10.5</t>
+          <t>Missouri State -3.5</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Illinois -12.8</t>
+          <t>Missouri State -5.9</t>
         </is>
       </c>
       <c r="I24" t="n">
-        <v>12.8</v>
+        <v>5.9</v>
       </c>
       <c r="J24" t="n">
-        <v>10.5</v>
+        <v>3.5</v>
       </c>
       <c r="K24" t="inlineStr"/>
       <c r="L24" t="inlineStr"/>
@@ -1716,40 +1716,40 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Boise State</t>
+          <t>Oregon State</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Fresno State</t>
+          <t>Washington State</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>5.4</v>
+        <v>5.9</v>
       </c>
       <c r="E26" t="n">
-        <v>2.199999999999999</v>
+        <v>2.3</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Boise State -17.5</t>
+          <t>Washington State -3.0</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Boise State -17.5</t>
+          <t>Washington State -3.5</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Boise State -19.7</t>
+          <t>Washington State -5.8</t>
         </is>
       </c>
       <c r="I26" t="n">
-        <v>19.7</v>
+        <v>-5.8</v>
       </c>
       <c r="J26" t="n">
-        <v>17.5</v>
+        <v>-3.5</v>
       </c>
       <c r="K26" t="inlineStr"/>
       <c r="L26" t="inlineStr"/>
@@ -1766,40 +1766,40 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Maryland</t>
+          <t>Boise State</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Indiana</t>
+          <t>Fresno State</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>7.5</v>
+        <v>5.4</v>
       </c>
       <c r="E27" t="n">
         <v>2.199999999999999</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Indiana -16.5</t>
+          <t>Boise State -17.5</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Indiana -22.5</t>
+          <t>Boise State -17.5</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Indiana -20.3</t>
+          <t>Boise State -19.7</t>
         </is>
       </c>
       <c r="I27" t="n">
-        <v>-20.3</v>
+        <v>19.7</v>
       </c>
       <c r="J27" t="n">
-        <v>-22.5</v>
+        <v>17.5</v>
       </c>
       <c r="K27" t="inlineStr"/>
       <c r="L27" t="inlineStr"/>
@@ -1816,40 +1816,40 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Colorado</t>
+          <t>Maryland</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Arizona</t>
+          <t>Indiana</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>8.300000000000001</v>
+        <v>7.5</v>
       </c>
       <c r="E28" t="n">
-        <v>2</v>
+        <v>2.199999999999999</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Arizona -4.5</t>
+          <t>Indiana -16.5</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Arizona -4.5</t>
+          <t>Indiana -22.5</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Arizona -2.5</t>
+          <t>Indiana -20.3</t>
         </is>
       </c>
       <c r="I28" t="n">
-        <v>-2.5</v>
+        <v>-20.3</v>
       </c>
       <c r="J28" t="n">
-        <v>-4.5</v>
+        <v>-22.5</v>
       </c>
       <c r="K28" t="inlineStr"/>
       <c r="L28" t="inlineStr"/>
@@ -1866,40 +1866,40 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Middle Tennessee</t>
+          <t>Western Kentucky</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Jacksonville State</t>
+          <t>New Mexico State</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>3.8</v>
+        <v>4.5</v>
       </c>
       <c r="E29" t="n">
-        <v>1.6</v>
+        <v>2.1</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Jacksonville State -6.5</t>
+          <t>Western Kentucky -9.5</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Jacksonville State -6</t>
+          <t>Western Kentucky -9.5</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Jacksonville State -7.6</t>
+          <t>Western Kentucky -11.6</t>
         </is>
       </c>
       <c r="I29" t="n">
-        <v>-7.6</v>
+        <v>11.6</v>
       </c>
       <c r="J29" t="n">
-        <v>-6</v>
+        <v>9.5</v>
       </c>
       <c r="K29" t="inlineStr"/>
       <c r="L29" t="inlineStr"/>
@@ -1916,40 +1916,40 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Minnesota</t>
+          <t>Virginia Tech</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Michigan State</t>
+          <t>Louisville</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>8.1</v>
+        <v>6.8</v>
       </c>
       <c r="E30" t="n">
-        <v>1.5</v>
+        <v>2.1</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Minnesota -5.5</t>
+          <t>Louisville -11.5</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>Minnesota -5.5</t>
+          <t>Louisville -10.5</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Minnesota -7.0</t>
+          <t>Louisville -12.6</t>
         </is>
       </c>
       <c r="I30" t="n">
-        <v>7</v>
+        <v>-12.6</v>
       </c>
       <c r="J30" t="n">
-        <v>5.5</v>
+        <v>-10.5</v>
       </c>
       <c r="K30" t="inlineStr"/>
       <c r="L30" t="inlineStr"/>
@@ -1966,37 +1966,37 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>UTSA</t>
+          <t>Colorado</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Tulane</t>
+          <t>Arizona</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>7.7</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="E31" t="n">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Tulane -3.5</t>
+          <t>Arizona -4.5</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Tulane -4.5</t>
+          <t>Arizona -4.5</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Tulane -3.0</t>
+          <t>Arizona -2.5</t>
         </is>
       </c>
       <c r="I31" t="n">
-        <v>-3</v>
+        <v>-2.5</v>
       </c>
       <c r="J31" t="n">
         <v>-4.5</v>
@@ -2016,40 +2016,40 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Stanford</t>
+          <t>San Diego State</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Pittsburgh</t>
+          <t>Wyoming</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>5.1</v>
+        <v>6.4</v>
       </c>
       <c r="E32" t="n">
-        <v>1.5</v>
+        <v>1.9</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Pittsburgh -15.5</t>
+          <t>San Diego State -10.0</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Pittsburgh -15.5</t>
+          <t>San Diego State -11.5</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Pittsburgh -17.0</t>
+          <t>San Diego State -13.4</t>
         </is>
       </c>
       <c r="I32" t="n">
-        <v>-17</v>
+        <v>13.4</v>
       </c>
       <c r="J32" t="n">
-        <v>-15.5</v>
+        <v>11.5</v>
       </c>
       <c r="K32" t="inlineStr"/>
       <c r="L32" t="inlineStr"/>
@@ -2066,40 +2066,40 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>SMU</t>
+          <t>Middle Tennessee</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>Jacksonville State</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>8.800000000000001</v>
+        <v>3.8</v>
       </c>
       <c r="E33" t="n">
-        <v>1.4</v>
+        <v>1.6</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Miami -1.5</t>
+          <t>Jacksonville State -6.5</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>Miami -10.5</t>
+          <t>Jacksonville State -6</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Miami -9.1</t>
+          <t>Jacksonville State -7.6</t>
         </is>
       </c>
       <c r="I33" t="n">
-        <v>-9.1</v>
+        <v>-7.6</v>
       </c>
       <c r="J33" t="n">
-        <v>-10.5</v>
+        <v>-6</v>
       </c>
       <c r="K33" t="inlineStr"/>
       <c r="L33" t="inlineStr"/>
@@ -2116,40 +2116,40 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>NC State</t>
+          <t>Ole Miss</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Georgia Tech</t>
+          <t>South Carolina</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>8.1</v>
+        <v>8.6</v>
       </c>
       <c r="E34" t="n">
-        <v>1.2</v>
+        <v>1.5</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Georgia Tech -4.5</t>
+          <t>Ole Miss -13.5</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Georgia Tech -6.5</t>
+          <t>Ole Miss -13.5</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Georgia Tech -7.7</t>
+          <t>Ole Miss -15.0</t>
         </is>
       </c>
       <c r="I34" t="n">
-        <v>-7.7</v>
+        <v>15</v>
       </c>
       <c r="J34" t="n">
-        <v>-6.5</v>
+        <v>13.5</v>
       </c>
       <c r="K34" t="inlineStr"/>
       <c r="L34" t="inlineStr"/>
@@ -2166,40 +2166,40 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Virginia Tech</t>
+          <t>Minnesota</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Louisville</t>
+          <t>Michigan State</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>6.8</v>
+        <v>8.1</v>
       </c>
       <c r="E35" t="n">
-        <v>1.1</v>
+        <v>1.5</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Louisville -11.5</t>
+          <t>Minnesota -5.5</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Louisville -11.5</t>
+          <t>Minnesota -5.5</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Louisville -12.6</t>
+          <t>Minnesota -7.0</t>
         </is>
       </c>
       <c r="I35" t="n">
-        <v>-12.6</v>
+        <v>7</v>
       </c>
       <c r="J35" t="n">
-        <v>-11.5</v>
+        <v>5.5</v>
       </c>
       <c r="K35" t="inlineStr"/>
       <c r="L35" t="inlineStr"/>
@@ -2216,40 +2216,40 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Clemson</t>
+          <t>UNLV</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Duke</t>
+          <t>New Mexico</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>9.199999999999999</v>
+        <v>7.6</v>
       </c>
       <c r="E36" t="n">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Clemson -3.5</t>
+          <t>UNLV -5.5</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>Clemson -3.5</t>
+          <t>UNLV -4.5</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Clemson -4.5</t>
+          <t>UNLV -6.0</t>
         </is>
       </c>
       <c r="I36" t="n">
+        <v>6</v>
+      </c>
+      <c r="J36" t="n">
         <v>4.5</v>
-      </c>
-      <c r="J36" t="n">
-        <v>3.5</v>
       </c>
       <c r="K36" t="inlineStr"/>
       <c r="L36" t="inlineStr"/>
@@ -2266,40 +2266,40 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Air Force</t>
+          <t>UTSA</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Army</t>
+          <t>Tulane</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>7</v>
+        <v>7.7</v>
       </c>
       <c r="E37" t="n">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Army -1.5</t>
+          <t>Tulane -3.5</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>Army -2.5</t>
+          <t>Tulane -4.5</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Army -1.5</t>
+          <t>Tulane -3.0</t>
         </is>
       </c>
       <c r="I37" t="n">
-        <v>-1.5</v>
+        <v>-3</v>
       </c>
       <c r="J37" t="n">
-        <v>-2.5</v>
+        <v>-4.5</v>
       </c>
       <c r="K37" t="inlineStr"/>
       <c r="L37" t="inlineStr"/>
@@ -2316,40 +2316,40 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Western Michigan</t>
+          <t>SMU</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Central Michigan</t>
+          <t>Miami</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>6.3</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="E38" t="n">
-        <v>0.5</v>
+        <v>1.4</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Western Michigan -6.0</t>
+          <t>Miami -1.5</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Western Michigan -6</t>
+          <t>Miami -10.5</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Western Michigan -6.5</t>
+          <t>Miami -9.1</t>
         </is>
       </c>
       <c r="I38" t="n">
-        <v>6.5</v>
+        <v>-9.1</v>
       </c>
       <c r="J38" t="n">
-        <v>6</v>
+        <v>-10.5</v>
       </c>
       <c r="K38" t="inlineStr"/>
       <c r="L38" t="inlineStr"/>
@@ -2366,40 +2366,40 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>UNLV</t>
+          <t>Nebraska</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>New Mexico</t>
+          <t>USC</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>7.6</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="E39" t="n">
-        <v>0.5</v>
+        <v>1.4</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>UNLV -5.5</t>
+          <t>USC -4.5</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>UNLV -5.5</t>
+          <t>USC -6</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>UNLV -6.0</t>
+          <t>USC -4.6</t>
         </is>
       </c>
       <c r="I39" t="n">
-        <v>6</v>
+        <v>-4.6</v>
       </c>
       <c r="J39" t="n">
-        <v>5.5</v>
+        <v>-6</v>
       </c>
       <c r="K39" t="inlineStr"/>
       <c r="L39" t="inlineStr"/>
@@ -2416,40 +2416,40 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>NC State</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>West Virginia</t>
+          <t>Georgia Tech</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>6.5</v>
+        <v>8.1</v>
       </c>
       <c r="E40" t="n">
-        <v>0.4000000000000004</v>
+        <v>1.2</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Houston -15.5</t>
+          <t>Georgia Tech -4.5</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>Houston -15.5</t>
+          <t>Georgia Tech -6.5</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Houston -15.1</t>
+          <t>Georgia Tech -7.7</t>
         </is>
       </c>
       <c r="I40" t="n">
-        <v>15.1</v>
+        <v>-7.7</v>
       </c>
       <c r="J40" t="n">
-        <v>15.5</v>
+        <v>-6.5</v>
       </c>
       <c r="K40" t="inlineStr"/>
       <c r="L40" t="inlineStr"/>
@@ -2466,40 +2466,40 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>South Alabama</t>
+          <t>Liberty</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Louisiana</t>
+          <t>Delaware</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>6.2</v>
+        <v>6.3</v>
       </c>
       <c r="E41" t="n">
-        <v>0.2999999999999998</v>
+        <v>1.1</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>South Alabama -4.5</t>
+          <t>Liberty -2.5</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>South Alabama -4.5</t>
+          <t>Liberty -3</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>South Alabama -4.8</t>
+          <t>Liberty -4.1</t>
         </is>
       </c>
       <c r="I41" t="n">
-        <v>4.8</v>
+        <v>4.1</v>
       </c>
       <c r="J41" t="n">
-        <v>4.5</v>
+        <v>3</v>
       </c>
       <c r="K41" t="inlineStr"/>
       <c r="L41" t="inlineStr"/>
@@ -2516,40 +2516,40 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Texas State</t>
+          <t>Kansas</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>James Madison</t>
+          <t>Oklahoma State</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>7</v>
+        <v>3.2</v>
       </c>
       <c r="E42" t="n">
-        <v>0.2000000000000002</v>
+        <v>1</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>James Madison -6.5</t>
+          <t>Kansas -24.5</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>James Madison -6.5</t>
+          <t>Kansas -25.5</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>James Madison -6.7</t>
+          <t>Kansas -26.5</t>
         </is>
       </c>
       <c r="I42" t="n">
-        <v>-6.7</v>
+        <v>26.5</v>
       </c>
       <c r="J42" t="n">
-        <v>-6.5</v>
+        <v>25.5</v>
       </c>
       <c r="K42" t="inlineStr"/>
       <c r="L42" t="inlineStr"/>
@@ -2566,40 +2566,40 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Temple</t>
+          <t>Clemson</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>East Carolina</t>
+          <t>Duke</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>7.2</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="E43" t="n">
-        <v>0.2000000000000002</v>
+        <v>1</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>East Carolina -4.5</t>
+          <t>Clemson -3.5</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>East Carolina -4.5</t>
+          <t>Clemson -3.5</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>East Carolina -4.7</t>
+          <t>Clemson -4.5</t>
         </is>
       </c>
       <c r="I43" t="n">
-        <v>-4.7</v>
+        <v>4.5</v>
       </c>
       <c r="J43" t="n">
-        <v>-4.5</v>
+        <v>3.5</v>
       </c>
       <c r="K43" t="inlineStr"/>
       <c r="L43" t="inlineStr"/>
@@ -2616,40 +2616,40 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Bowling Green</t>
+          <t>Arkansas</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Buffalo</t>
+          <t>Mississippi State</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>6.1</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="E44" t="n">
-        <v>0.2</v>
+        <v>0.9000000000000004</v>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Bowling Green -1.5</t>
+          <t>Arkansas -3.5</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>Bowling Green -1.5</t>
+          <t>Arkansas -3.5</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Bowling Green -1.7</t>
+          <t>Arkansas -4.4</t>
         </is>
       </c>
       <c r="I44" t="n">
-        <v>1.7</v>
+        <v>4.4</v>
       </c>
       <c r="J44" t="n">
-        <v>1.5</v>
+        <v>3.5</v>
       </c>
       <c r="K44" t="inlineStr"/>
       <c r="L44" t="inlineStr"/>
@@ -2666,40 +2666,40 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Nebraska</t>
+          <t>South Alabama</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>USC</t>
+          <t>Louisiana</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>9.300000000000001</v>
+        <v>6.2</v>
       </c>
       <c r="E45" t="n">
-        <v>0.09999999999999964</v>
+        <v>0.7999999999999998</v>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>USC -4.5</t>
+          <t>South Alabama -4.5</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>USC -4.5</t>
+          <t>South Alabama -4</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>USC -4.6</t>
+          <t>South Alabama -4.8</t>
         </is>
       </c>
       <c r="I45" t="n">
-        <v>-4.6</v>
+        <v>4.8</v>
       </c>
       <c r="J45" t="n">
-        <v>-4.5</v>
+        <v>4</v>
       </c>
       <c r="K45" t="inlineStr"/>
       <c r="L45" t="inlineStr"/>
@@ -2710,6 +2710,406 @@
         <v>0</v>
       </c>
     </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Houston</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>West Virginia</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="E46" t="n">
+        <v>0.4000000000000004</v>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>Houston -15.5</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>Houston -15.5</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>Houston -15.1</t>
+        </is>
+      </c>
+      <c r="I46" t="n">
+        <v>15.1</v>
+      </c>
+      <c r="J46" t="n">
+        <v>15.5</v>
+      </c>
+      <c r="K46" t="inlineStr"/>
+      <c r="L46" t="inlineStr"/>
+      <c r="M46" t="inlineStr"/>
+      <c r="N46" t="inlineStr"/>
+      <c r="O46" t="inlineStr"/>
+      <c r="P46" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Illinois</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Rutgers</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>8.1</v>
+      </c>
+      <c r="E47" t="n">
+        <v>0.3000000000000007</v>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>Illinois -10.5</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>Illinois -12.5</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>Illinois -12.8</t>
+        </is>
+      </c>
+      <c r="I47" t="n">
+        <v>12.8</v>
+      </c>
+      <c r="J47" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="K47" t="inlineStr"/>
+      <c r="L47" t="inlineStr"/>
+      <c r="M47" t="inlineStr"/>
+      <c r="N47" t="inlineStr"/>
+      <c r="O47" t="inlineStr"/>
+      <c r="P47" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Texas State</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>James Madison</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>7</v>
+      </c>
+      <c r="E48" t="n">
+        <v>0.2000000000000002</v>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>James Madison -6.5</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>James Madison -6.5</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>James Madison -6.7</t>
+        </is>
+      </c>
+      <c r="I48" t="n">
+        <v>-6.7</v>
+      </c>
+      <c r="J48" t="n">
+        <v>-6.5</v>
+      </c>
+      <c r="K48" t="inlineStr"/>
+      <c r="L48" t="inlineStr"/>
+      <c r="M48" t="inlineStr"/>
+      <c r="N48" t="inlineStr"/>
+      <c r="O48" t="inlineStr"/>
+      <c r="P48" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Temple</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>East Carolina</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>7.2</v>
+      </c>
+      <c r="E49" t="n">
+        <v>0.2000000000000002</v>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>East Carolina -4.5</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>East Carolina -4.5</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>East Carolina -4.7</t>
+        </is>
+      </c>
+      <c r="I49" t="n">
+        <v>-4.7</v>
+      </c>
+      <c r="J49" t="n">
+        <v>-4.5</v>
+      </c>
+      <c r="K49" t="inlineStr"/>
+      <c r="L49" t="inlineStr"/>
+      <c r="M49" t="inlineStr"/>
+      <c r="N49" t="inlineStr"/>
+      <c r="O49" t="inlineStr"/>
+      <c r="P49" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Bowling Green</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Buffalo</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>6.1</v>
+      </c>
+      <c r="E50" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>Bowling Green -1.5</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>Bowling Green -1.5</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>Bowling Green -1.7</t>
+        </is>
+      </c>
+      <c r="I50" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="J50" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="K50" t="inlineStr"/>
+      <c r="L50" t="inlineStr"/>
+      <c r="M50" t="inlineStr"/>
+      <c r="N50" t="inlineStr"/>
+      <c r="O50" t="inlineStr"/>
+      <c r="P50" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Western Michigan</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Central Michigan</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>6.3</v>
+      </c>
+      <c r="E51" t="n">
+        <v>0</v>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>Western Michigan -6.0</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>Western Michigan -6.5</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>Western Michigan -6.5</t>
+        </is>
+      </c>
+      <c r="I51" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="J51" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="K51" t="inlineStr"/>
+      <c r="L51" t="inlineStr"/>
+      <c r="M51" t="inlineStr"/>
+      <c r="N51" t="inlineStr"/>
+      <c r="O51" t="inlineStr"/>
+      <c r="P51" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>San José State</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Hawai'i</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>7</v>
+      </c>
+      <c r="E52" t="n">
+        <v>0</v>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>San José State -1.5</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>San José State -1.5</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>San José State -1.5</t>
+        </is>
+      </c>
+      <c r="I52" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="J52" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="K52" t="inlineStr"/>
+      <c r="L52" t="inlineStr"/>
+      <c r="M52" t="inlineStr"/>
+      <c r="N52" t="inlineStr"/>
+      <c r="O52" t="inlineStr"/>
+      <c r="P52" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Air Force</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Army</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>7</v>
+      </c>
+      <c r="E53" t="n">
+        <v>0</v>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>Army -1.5</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>Army -1.5</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>Army -1.5</t>
+        </is>
+      </c>
+      <c r="I53" t="n">
+        <v>-1.5</v>
+      </c>
+      <c r="J53" t="n">
+        <v>-1.5</v>
+      </c>
+      <c r="K53" t="inlineStr"/>
+      <c r="L53" t="inlineStr"/>
+      <c r="M53" t="inlineStr"/>
+      <c r="N53" t="inlineStr"/>
+      <c r="O53" t="inlineStr"/>
+      <c r="P53" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
trying to show outlet
</commit_message>
<xml_diff>
--- a/PEAR/PEAR Football/y2025/Spreads/spreads_tracker_week10.xlsx
+++ b/PEAR/PEAR Football/y2025/Spreads/spreads_tracker_week10.xlsx
@@ -2896,7 +2896,11 @@
           <t>2:00 PM</t>
         </is>
       </c>
-      <c r="D34" t="inlineStr"/>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
       <c r="E34" t="inlineStr">
         <is>
           <t>UNLV</t>

</xml_diff>